<commit_message>
Images of results and tables
</commit_message>
<xml_diff>
--- a/Tables examples/speaking-example.xlsx
+++ b/Tables examples/speaking-example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CardMaker-Pro\Tables test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CardMaker-Pro\Tables examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8473609-145E-45DA-9DAD-98B7314F49DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3995BA9-7388-4002-90BC-AADCF8915555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>¿Qué resultados pretendes encontrar con esta investigación?</t>
   </si>
@@ -46,90 +46,6 @@
   </si>
   <si>
     <t>¡Esta película es tan aburrida!</t>
-  </si>
-  <si>
-    <t>La regresión polinomial se ajusta a una relación no lineal entre el valor de X</t>
-  </si>
-  <si>
-    <t> Por esta razón, la regresión polinomial se considera un caso especial de regresión lineal múltiple.</t>
-  </si>
-  <si>
-    <t> Por lo tanto, para el análisis de mínimos cuadrados</t>
-  </si>
-  <si>
-    <t>Esta pizza es más pequeña de lo que esperaba.</t>
-  </si>
-  <si>
-    <t>con un doble subíndice donde el primero indica la fila y el segundo la columna a la que pertenece.</t>
-  </si>
-  <si>
-    <r>
-      <t>En </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF0645AD"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>matemática</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, una </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>matriz</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> es un conjunto </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF0645AD"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>bidimensional</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> de </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF0645AD"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>números</t>
-    </r>
   </si>
   <si>
     <t>Speaking</t>
@@ -139,7 +55,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,25 +76,12 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF0645AD"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF202122"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -200,13 +103,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -491,17 +394,17 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A14" sqref="A9:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="59.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" x14ac:dyDescent="0.35">
@@ -540,41 +443,25 @@
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A9" s="2"/>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="A10" s="3"/>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="A11" s="3"/>
     </row>
     <row r="12" spans="1:1" ht="15" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A12" s="1"/>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A13" s="2"/>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="A14" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A10" r:id="rId1" tooltip="Regresión lineal" display="https://es.wikipedia.org/wiki/Regresi%C3%B3n_lineal" xr:uid="{FDA1A12F-19AD-41F6-BAAC-FBDAAEB5D73A}"/>
-    <hyperlink ref="A11" r:id="rId2" tooltip="Mínimos cuadrados" display="https://es.wikipedia.org/wiki/M%C3%ADnimos_cuadrados" xr:uid="{D7B6287F-189D-4009-B5DB-70C3027EBF67}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added audios inside anki deck
</commit_message>
<xml_diff>
--- a/Tables examples/speaking-example.xlsx
+++ b/Tables examples/speaking-example.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Speaking</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>La historia era mi asignatura favorita en el colegio.</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Estoy en mi cuarto curso en la facultad de medicina</t>
@@ -54,7 +51,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,22 +60,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF202122"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -109,25 +99,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -154,28 +135,28 @@
         <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F818D"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -431,17 +412,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="59.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="48.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="7.2907142857142855" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,7 +430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -457,77 +438,41 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
+      <c r="B8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>